<commit_message>
Initial commit - SSL 설문조사 시스템 with JSON support
</commit_message>
<xml_diff>
--- a/docs/MRT_stu_codes_0515.xlsx
+++ b/docs/MRT_stu_codes_0515.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yoonj\OneDrive\바탕 화면\To do\Survey_0516_mod\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lhc48\ssl-survey-0516\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F57715D-C23F-4BEE-93BA-F1D5B9133850}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08F242BE-B5C6-4CD3-A337-FF98FF94D0D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3290" yWindow="2940" windowWidth="19200" windowHeight="9970" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Recent" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="62">
   <si>
     <t>code</t>
   </si>
@@ -198,6 +198,22 @@
   <si>
     <t>MRTKfcu</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TEST101</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TEST102</t>
+  </si>
+  <si>
+    <t>TEST103</t>
+  </si>
+  <si>
+    <t>TEST104</t>
+  </si>
+  <si>
+    <t>TEST105</t>
   </si>
 </sst>
 </file>
@@ -591,259 +607,259 @@
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -856,267 +872,292 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:A51"/>
+  <dimension ref="A1:A56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A28" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A29" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A30" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A31" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A32" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A33" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A34" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A35" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A36" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A37" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A38" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A39" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A40" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A41" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A42" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A43" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A44" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A45" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A46" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A47" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A48" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.6">
-      <c r="A49" s="3" t="s">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A49" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.6">
-      <c r="A50" s="3" t="s">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A50" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A51" s="2" t="s">
         <v>56</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A52" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A53" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A54" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A55" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A56" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>